<commit_message>
updates after discussion with Emma.
</commit_message>
<xml_diff>
--- a/tabular/drug_resistance/drugResistanceFindings.xlsx
+++ b/tabular/drug_resistance/drugResistanceFindings.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-28500" yWindow="1960" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="12000" yWindow="6760" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
-  <si>
-    <t>Lenz_et_al_2010</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t>Drug</t>
   </si>
@@ -30,9 +27,6 @@
     <t>PublicationID</t>
   </si>
   <si>
-    <t>Simeprevir</t>
-  </si>
-  <si>
     <t>Gene</t>
   </si>
   <si>
@@ -45,9 +39,6 @@
     <t>NS3</t>
   </si>
   <si>
-    <t>80R+168A</t>
-  </si>
-  <si>
     <t>in_vitro</t>
   </si>
   <si>
@@ -64,13 +55,31 @@
   </si>
   <si>
     <t>Substitutions</t>
+  </si>
+  <si>
+    <t>Lenz_et_al_2013</t>
+  </si>
+  <si>
+    <t>168Q</t>
+  </si>
+  <si>
+    <t>clinical</t>
+  </si>
+  <si>
+    <t>3a</t>
+  </si>
+  <si>
+    <t>simeprevir</t>
+  </si>
+  <si>
+    <t>SVR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -82,6 +91,14 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -104,15 +121,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -442,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -456,56 +477,82 @@
     <col min="6" max="6" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
         <v>14</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="F3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2">
-        <v>2655</v>
+      <c r="H3">
+        <v>385</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
various tweaks relating to sorting and linking.
</commit_message>
<xml_diff>
--- a/tabular/drug_resistance/drugResistanceFindings.xlsx
+++ b/tabular/drug_resistance/drugResistanceFindings.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="12000" yWindow="6760" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="20840" yWindow="7580" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="50">
   <si>
     <t>Drug</t>
   </si>
@@ -73,6 +73,102 @@
   </si>
   <si>
     <t>SVR</t>
+  </si>
+  <si>
+    <t>36L+80K</t>
+  </si>
+  <si>
+    <t>80K</t>
+  </si>
+  <si>
+    <t>S122R</t>
+  </si>
+  <si>
+    <t>36L+80K+122T</t>
+  </si>
+  <si>
+    <t>36L</t>
+  </si>
+  <si>
+    <t>36M</t>
+  </si>
+  <si>
+    <t>36A</t>
+  </si>
+  <si>
+    <t>41R</t>
+  </si>
+  <si>
+    <t>43S</t>
+  </si>
+  <si>
+    <t>54A</t>
+  </si>
+  <si>
+    <t>54S</t>
+  </si>
+  <si>
+    <t>80R</t>
+  </si>
+  <si>
+    <t>80H</t>
+  </si>
+  <si>
+    <t>80G</t>
+  </si>
+  <si>
+    <t>155Q</t>
+  </si>
+  <si>
+    <t>155T</t>
+  </si>
+  <si>
+    <t>155K</t>
+  </si>
+  <si>
+    <t>155G</t>
+  </si>
+  <si>
+    <t>156S</t>
+  </si>
+  <si>
+    <t>156G</t>
+  </si>
+  <si>
+    <t>156T</t>
+  </si>
+  <si>
+    <t>156V</t>
+  </si>
+  <si>
+    <t>168G</t>
+  </si>
+  <si>
+    <t>168E</t>
+  </si>
+  <si>
+    <t>168T</t>
+  </si>
+  <si>
+    <t>168Y</t>
+  </si>
+  <si>
+    <t>168H</t>
+  </si>
+  <si>
+    <t>168A</t>
+  </si>
+  <si>
+    <t>168V</t>
+  </si>
+  <si>
+    <t>170T</t>
+  </si>
+  <si>
+    <t>80K+155K</t>
+  </si>
+  <si>
+    <t>Lenz_et_al_2010</t>
   </si>
 </sst>
 </file>
@@ -121,8 +217,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -130,10 +250,34 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="28">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -463,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36:XFD36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -555,6 +699,838 @@
         <v>385</v>
       </c>
     </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" t="s">
+        <v>8</v>
+      </c>
+      <c r="H16">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" t="s">
+        <v>7</v>
+      </c>
+      <c r="G17" t="s">
+        <v>8</v>
+      </c>
+      <c r="H17">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" t="s">
+        <v>7</v>
+      </c>
+      <c r="G18" t="s">
+        <v>8</v>
+      </c>
+      <c r="H18">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F19" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" t="s">
+        <v>8</v>
+      </c>
+      <c r="H19">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" t="s">
+        <v>6</v>
+      </c>
+      <c r="F20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G20" t="s">
+        <v>8</v>
+      </c>
+      <c r="H20">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21" t="s">
+        <v>6</v>
+      </c>
+      <c r="F21" t="s">
+        <v>7</v>
+      </c>
+      <c r="G21" t="s">
+        <v>8</v>
+      </c>
+      <c r="H21">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" t="s">
+        <v>35</v>
+      </c>
+      <c r="E22" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22" t="s">
+        <v>8</v>
+      </c>
+      <c r="H22">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" t="s">
+        <v>36</v>
+      </c>
+      <c r="E23" t="s">
+        <v>6</v>
+      </c>
+      <c r="F23" t="s">
+        <v>7</v>
+      </c>
+      <c r="G23" t="s">
+        <v>8</v>
+      </c>
+      <c r="H23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" t="s">
+        <v>37</v>
+      </c>
+      <c r="E24" t="s">
+        <v>6</v>
+      </c>
+      <c r="F24" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24" t="s">
+        <v>8</v>
+      </c>
+      <c r="H24">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" t="s">
+        <v>38</v>
+      </c>
+      <c r="E25" t="s">
+        <v>6</v>
+      </c>
+      <c r="F25" t="s">
+        <v>7</v>
+      </c>
+      <c r="G25" t="s">
+        <v>8</v>
+      </c>
+      <c r="H25">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" t="s">
+        <v>39</v>
+      </c>
+      <c r="E26" t="s">
+        <v>6</v>
+      </c>
+      <c r="F26" t="s">
+        <v>7</v>
+      </c>
+      <c r="G26" t="s">
+        <v>8</v>
+      </c>
+      <c r="H26">
+        <v>2149</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" t="s">
+        <v>40</v>
+      </c>
+      <c r="E27" t="s">
+        <v>6</v>
+      </c>
+      <c r="F27" t="s">
+        <v>7</v>
+      </c>
+      <c r="G27" t="s">
+        <v>8</v>
+      </c>
+      <c r="H27">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" t="s">
+        <v>41</v>
+      </c>
+      <c r="E28" t="s">
+        <v>6</v>
+      </c>
+      <c r="F28" t="s">
+        <v>7</v>
+      </c>
+      <c r="G28" t="s">
+        <v>8</v>
+      </c>
+      <c r="H28">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" t="s">
+        <v>42</v>
+      </c>
+      <c r="E29" t="s">
+        <v>6</v>
+      </c>
+      <c r="F29" t="s">
+        <v>7</v>
+      </c>
+      <c r="G29" t="s">
+        <v>8</v>
+      </c>
+      <c r="H29">
+        <v>4089</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" t="s">
+        <v>49</v>
+      </c>
+      <c r="C30" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" t="s">
+        <v>43</v>
+      </c>
+      <c r="E30" t="s">
+        <v>6</v>
+      </c>
+      <c r="F30" t="s">
+        <v>7</v>
+      </c>
+      <c r="G30" t="s">
+        <v>8</v>
+      </c>
+      <c r="H30">
+        <v>6238</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31" t="s">
+        <v>49</v>
+      </c>
+      <c r="C31" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" t="s">
+        <v>44</v>
+      </c>
+      <c r="E31" t="s">
+        <v>6</v>
+      </c>
+      <c r="F31" t="s">
+        <v>7</v>
+      </c>
+      <c r="G31" t="s">
+        <v>8</v>
+      </c>
+      <c r="H31">
+        <v>5655</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" t="s">
+        <v>49</v>
+      </c>
+      <c r="C32" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" t="s">
+        <v>45</v>
+      </c>
+      <c r="E32" t="s">
+        <v>6</v>
+      </c>
+      <c r="F32" t="s">
+        <v>7</v>
+      </c>
+      <c r="G32" t="s">
+        <v>8</v>
+      </c>
+      <c r="H32">
+        <v>6356</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33" t="s">
+        <v>49</v>
+      </c>
+      <c r="C33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" t="s">
+        <v>46</v>
+      </c>
+      <c r="E33" t="s">
+        <v>6</v>
+      </c>
+      <c r="F33" t="s">
+        <v>7</v>
+      </c>
+      <c r="G33" t="s">
+        <v>8</v>
+      </c>
+      <c r="H33">
+        <v>17917</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" t="s">
+        <v>16</v>
+      </c>
+      <c r="B34" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" t="s">
+        <v>47</v>
+      </c>
+      <c r="E34" t="s">
+        <v>6</v>
+      </c>
+      <c r="F34" t="s">
+        <v>7</v>
+      </c>
+      <c r="G34" t="s">
+        <v>8</v>
+      </c>
+      <c r="H34">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35" t="s">
+        <v>49</v>
+      </c>
+      <c r="C35" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" t="s">
+        <v>48</v>
+      </c>
+      <c r="E35" t="s">
+        <v>6</v>
+      </c>
+      <c r="F35" t="s">
+        <v>7</v>
+      </c>
+      <c r="G35" t="s">
+        <v>8</v>
+      </c>
+      <c r="H35">
+        <v>4647</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>